<commit_message>
Before starting to build the search returner
</commit_message>
<xml_diff>
--- a/iss_template.xlsx
+++ b/iss_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\gnarfle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1130084D-3E95-4A0D-8525-8BE2D6E1054F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACA0CD3-564B-45CC-AFDE-DB6793A9C4DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18096" yWindow="168" windowWidth="17280" windowHeight="9468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iss_template" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>search_run_date</t>
   </si>
   <si>
-    <t>pizza+delivery</t>
+    <t>delivery+person</t>
   </si>
 </sst>
 </file>
@@ -895,11 +895,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -929,7 +930,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">NOW()</f>
-        <v>43719.314907870372</v>
+        <v>43719.337774652777</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -944,7 +945,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">NOW()</f>
-        <v>43719.314907870372</v>
+        <v>43719.337774652777</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -959,7 +960,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43719.314907870372</v>
+        <v>43719.337774652777</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -974,7 +975,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>43719.314907870372</v>
+        <v>43719.337774652777</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>

</xml_diff>